<commit_message>
The classroom information deleted when time out
结束时间到了自动删除班级有关的信息的功能完成。
</commit_message>
<xml_diff>
--- a/docs/工作内容.xlsx
+++ b/docs/工作内容.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>任务编号</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -133,59 +133,67 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
+    <t>服务器端进行信息的中转的时候不应该使用对方的ip进行信息的传输，而应该使用收到的socket进行通信</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用两个socket进行通信，一个用于接收，一个用于发送</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用两个socket进行通信，一个用于接收，一个用于发送</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>根据register的内容对客户端的SharedPreferences和相关的内容进行修改</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>一个蓝牙只能创建一个教室，客户端在创建教室失败时，做出相应的提示！</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>通过json处理将客户端的发过来的json信息（信息类型+教室号）进行分解，并根据信息类型进行不同的处理</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>当客户端收到签到的消息，自动弹出签到框</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>将半双工的socket通信变成了全双工的socket的通信，之前的通过IP地址广播的方式完全修改了</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>课程的id需要从客户端传来数据</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成classmates表对应的dao</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成整个签到流程</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>1 2</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>服务器端进行信息的中转的时候不应该使用对方的ip进行信息的传输，而应该使用收到的socket进行通信</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用两个socket进行通信，一个用于接收，一个用于发送</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用两个socket进行通信，一个用于接收，一个用于发送</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>根据register的内容对客户端的SharedPreferences和相关的内容进行修改</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>一个蓝牙只能创建一个教室，客户端在创建教室失败时，做出相应的提示！</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>通过json处理将客户端的发过来的json信息（信息类型+教室号）进行分解，并根据信息类型进行不同的处理</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>当客户端收到签到的消息，自动弹出签到框</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>将半双工的socket通信变成了全双工的socket的通信，之前的通过IP地址广播的方式完全修改了</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>课程的id需要从客户端传来数据</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成classmates表对应的dao</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成整个签到流程</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1 2</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>获得签到文件功能</t>
+    <t>使用FTP在服务器端建立服务器，是应用可以通过url进行下载</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用DownloadManager进行下载，下载后的文件存入下载管理中</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>在客户单创建线程，对创建的教室进行计时，超时后想服务器端发指令</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>服务器端创建一个管理超时的</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -261,7 +269,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -274,9 +282,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
@@ -616,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -758,7 +763,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D8" s="3">
         <v>1</v>
@@ -911,7 +916,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="3">
         <v>1</v>
@@ -928,7 +933,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="3">
         <v>1</v>
@@ -1013,7 +1018,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" s="3">
         <v>1</v>
@@ -1030,7 +1035,7 @@
         <v>1</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D24" s="3">
         <v>1</v>
@@ -1064,7 +1069,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D26" s="3">
         <v>1</v>
@@ -1081,7 +1086,7 @@
         <v>1</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27" s="3">
         <v>1</v>
@@ -1098,7 +1103,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D28" s="3">
         <v>1</v>
@@ -1115,7 +1120,7 @@
         <v>2</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D29" s="3">
         <v>1</v>
@@ -1129,10 +1134,10 @@
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D30" s="3">
         <v>1</v>
@@ -1145,40 +1150,70 @@
       <c r="A31" s="3">
         <v>30</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>42</v>
+      <c r="B31" s="3">
+        <v>2</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="D31" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" s="3">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B32" s="3">
+        <v>1</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1</v>
+      </c>
+      <c r="E32" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" s="3">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B33" s="3">
+        <v>1</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1</v>
+      </c>
+      <c r="E33" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" s="3">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="B34" s="3">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" s="3">
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -1232,8 +1267,8 @@
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>30</v>
+      <c r="B4" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">

</xml_diff>